<commit_message>
updates to data regarding fuel and ship costs
</commit_message>
<xml_diff>
--- a/data/ship_eff+transportwork.xlsx
+++ b/data/ship_eff+transportwork.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
   <si>
     <t>Average transport work per ship type</t>
   </si>
@@ -196,24 +196,6 @@
     <t>Container</t>
   </si>
   <si>
-    <t>0-999</t>
-  </si>
-  <si>
-    <t>1000-1999</t>
-  </si>
-  <si>
-    <t>2000-2999</t>
-  </si>
-  <si>
-    <t>3000-4999</t>
-  </si>
-  <si>
-    <t>5000-7999</t>
-  </si>
-  <si>
-    <t>8000+</t>
-  </si>
-  <si>
     <t>ton-NM</t>
   </si>
   <si>
@@ -223,58 +205,40 @@
     <t>Bulk carrier</t>
   </si>
   <si>
-    <t>0-9999</t>
-  </si>
-  <si>
-    <t>10000-34999</t>
-  </si>
-  <si>
-    <t>35000-59999</t>
-  </si>
-  <si>
-    <t>60000-99999</t>
-  </si>
-  <si>
-    <t>100000-199999</t>
-  </si>
-  <si>
-    <t>200000+</t>
-  </si>
-  <si>
-    <t>general cargo</t>
-  </si>
-  <si>
-    <t>0-4999</t>
-  </si>
-  <si>
-    <t>5000-9999</t>
-  </si>
-  <si>
-    <t>10000+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bulk </t>
-  </si>
-  <si>
-    <t>rough average size</t>
-  </si>
-  <si>
-    <t>3000 TEU</t>
-  </si>
-  <si>
-    <t>*based on table 9.1 and table 72 and 73</t>
-  </si>
-  <si>
-    <t>80000 dwt</t>
-  </si>
-  <si>
-    <t>panamax</t>
-  </si>
-  <si>
     <t>NHG</t>
   </si>
   <si>
     <t>NHB</t>
+  </si>
+  <si>
+    <t>Third IMO study 2014</t>
+  </si>
+  <si>
+    <t>oil tanker</t>
+  </si>
+  <si>
+    <t>General cargo</t>
+  </si>
+  <si>
+    <t>dwt</t>
+  </si>
+  <si>
+    <t>teu</t>
+  </si>
+  <si>
+    <t>active IHSF</t>
+  </si>
+  <si>
+    <t>average dwt</t>
+  </si>
+  <si>
+    <t>average installed power kW</t>
+  </si>
+  <si>
+    <t>average teu</t>
+  </si>
+  <si>
+    <t>average over size</t>
   </si>
 </sst>
 </file>
@@ -329,7 +293,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
@@ -340,6 +304,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,13 +329,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>55034</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>370771</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>54677</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -400,16 +365,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>392642</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>140758</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>43392</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>172508</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>315766</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>25448</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>580349</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>57198</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -426,46 +391,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13367809" y="140758"/>
+          <a:off x="16553392" y="363008"/>
           <a:ext cx="5447624" cy="8076190"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>275167</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>105833</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>109357</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>124119</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7408334" y="3915833"/>
-          <a:ext cx="5676190" cy="6114286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -935,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AJ110"/>
+  <dimension ref="A2:AK115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="P41" sqref="P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,12 +877,13 @@
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I2">
         <v>1</v>
       </c>
@@ -963,7 +891,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -974,16 +902,19 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>53</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="M4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>63</v>
+      </c>
+      <c r="N4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -999,17 +930,23 @@
       <c r="F5" t="s">
         <v>5</v>
       </c>
+      <c r="K5" t="s">
+        <v>67</v>
+      </c>
       <c r="L5" t="s">
-        <v>64</v>
-      </c>
-      <c r="M5">
+        <v>67</v>
+      </c>
+      <c r="M5" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5">
         <v>2012</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>2050</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -1025,41 +962,44 @@
       <c r="F6" s="3">
         <v>0.3</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K6" t="s">
-        <v>58</v>
-      </c>
-      <c r="L6" s="5">
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>999</v>
+      </c>
+      <c r="M6" s="5">
         <v>179809363</v>
       </c>
-      <c r="M6" s="7">
+      <c r="N6" s="7">
         <v>0.22</v>
       </c>
-      <c r="N6">
-        <f>+L6*M6</f>
+      <c r="O6">
+        <f>+M6*N6</f>
         <v>39558059.859999999</v>
       </c>
-      <c r="O6" s="8">
+      <c r="P6" s="8">
         <v>0.22</v>
       </c>
-      <c r="P6">
-        <f>+L6*O6</f>
+      <c r="Q6">
+        <f>+M6*P6</f>
         <v>39558059.859999999</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <f>+B6*$I$3</f>
         <v>5.556</v>
       </c>
       <c r="C7" s="4">
-        <f t="shared" ref="C7:F7" si="0">+C6*$I$3</f>
+        <f>+C6*$I$3</f>
         <v>12.964</v>
       </c>
       <c r="D7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C7:F7" si="0">+D6*$I$3</f>
         <v>0.92600000000000005</v>
       </c>
       <c r="E7" s="4">
@@ -1070,28 +1010,31 @@
         <f t="shared" si="0"/>
         <v>0.55559999999999998</v>
       </c>
-      <c r="K7" t="s">
-        <v>59</v>
-      </c>
-      <c r="L7" s="5">
+      <c r="K7">
+        <v>1000</v>
+      </c>
+      <c r="L7">
+        <v>1999</v>
+      </c>
+      <c r="M7" s="5">
         <v>578339367</v>
       </c>
-      <c r="M7" s="8">
+      <c r="N7" s="8">
         <v>0.25</v>
       </c>
-      <c r="N7">
-        <f t="shared" ref="N7:N15" si="1">+L7*M7</f>
+      <c r="O7">
+        <f t="shared" ref="O7:O9" si="1">+M7*N7</f>
         <v>144584841.75</v>
       </c>
-      <c r="O7" s="8">
+      <c r="P7" s="8">
         <v>0.2</v>
       </c>
-      <c r="P7">
-        <f t="shared" ref="P7:P17" si="2">+L7*O7</f>
+      <c r="Q7">
+        <f t="shared" ref="Q7:Q20" si="2">+M7*P7</f>
         <v>115667873.40000001</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2012</v>
       </c>
@@ -1099,35 +1042,38 @@
         <v>7000000000</v>
       </c>
       <c r="C8" s="5">
-        <f>+SUM(N12:N17)</f>
+        <f>+SUM(O17:O22)</f>
         <v>5207608850.96</v>
       </c>
       <c r="E8" s="5">
-        <f>+SUM(N6:N11)</f>
-        <v>2033999167.0539999</v>
-      </c>
-      <c r="K8" t="s">
-        <v>60</v>
-      </c>
-      <c r="L8" s="5">
+        <f>+SUM(O6:O13)</f>
+        <v>2033999167.0540001</v>
+      </c>
+      <c r="K8">
+        <v>2000</v>
+      </c>
+      <c r="L8">
+        <v>2999</v>
+      </c>
+      <c r="M8" s="5">
         <v>1480205694</v>
       </c>
-      <c r="M8" s="8">
+      <c r="N8" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <f t="shared" si="1"/>
         <v>207228797.16000003</v>
       </c>
-      <c r="O8" s="8">
+      <c r="P8" s="8">
         <v>0.18</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <f t="shared" si="2"/>
         <v>266437024.91999999</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2050</v>
       </c>
@@ -1135,35 +1081,38 @@
         <v>7000000000</v>
       </c>
       <c r="C9" s="5">
-        <f>+SUM(P12:P17)</f>
+        <f>+SUM(Q17:Q22)</f>
         <v>5599732634.3800001</v>
       </c>
       <c r="E9" s="5">
-        <f>+SUM(P6:P11)</f>
-        <v>2700751170.8000002</v>
-      </c>
-      <c r="K9" t="s">
-        <v>61</v>
-      </c>
-      <c r="L9" s="5">
+        <f>+SUM(Q6:Q13)</f>
+        <v>2700751170.7999997</v>
+      </c>
+      <c r="K9">
+        <v>3000</v>
+      </c>
+      <c r="L9">
+        <v>4999</v>
+      </c>
+      <c r="M9" s="5">
         <v>2820323533</v>
       </c>
-      <c r="M9" s="8">
+      <c r="N9" s="8">
         <v>0.19</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <f t="shared" si="1"/>
         <v>535861471.26999998</v>
       </c>
-      <c r="O9" s="8">
+      <c r="P9" s="8">
         <v>0.05</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <f t="shared" si="2"/>
         <v>141016176.65000001</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2012</v>
       </c>
@@ -1179,28 +1128,31 @@
         <f>+E8/1000000000</f>
         <v>2.0339991670540001</v>
       </c>
-      <c r="K10" t="s">
-        <v>62</v>
-      </c>
-      <c r="L10" s="5">
+      <c r="K10">
+        <v>5000</v>
+      </c>
+      <c r="L10">
+        <v>7999</v>
+      </c>
+      <c r="M10" s="5">
         <v>4233489679</v>
       </c>
-      <c r="M10" s="8">
+      <c r="N10" s="8">
         <v>0.11</v>
       </c>
-      <c r="N10">
-        <f t="shared" si="1"/>
+      <c r="O10">
+        <f>+M10*N10</f>
         <v>465683864.69</v>
       </c>
-      <c r="O10" s="8">
+      <c r="P10" s="8">
         <v>0.11</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <f t="shared" si="2"/>
         <v>465683864.69</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2050</v>
       </c>
@@ -1214,423 +1166,586 @@
       </c>
       <c r="E11" s="9">
         <f>+E9/1000000000</f>
-        <v>2.7007511708000003</v>
-      </c>
-      <c r="K11" t="s">
-        <v>63</v>
-      </c>
-      <c r="L11" s="5">
+        <v>2.7007511707999998</v>
+      </c>
+      <c r="K11">
+        <v>8000</v>
+      </c>
+      <c r="L11">
+        <v>11999</v>
+      </c>
+      <c r="M11" s="5">
         <v>6968284047</v>
       </c>
-      <c r="M11" s="8">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="1"/>
-        <v>641082132.324</v>
-      </c>
-      <c r="O11" s="8">
-        <v>0.24</v>
-      </c>
-      <c r="P11">
+      <c r="N11" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O11">
+        <f>+M11*N11</f>
+        <v>487779883.29000002</v>
+      </c>
+      <c r="P11" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="Q11">
         <f t="shared" si="2"/>
-        <v>1672388171.28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" t="s">
-        <v>79</v>
-      </c>
-      <c r="J12" t="s">
+        <v>696828404.70000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>12000</v>
+      </c>
+      <c r="L12">
+        <v>14500</v>
+      </c>
+      <c r="M12" s="5">
+        <v>6968284047</v>
+      </c>
+      <c r="N12" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ref="O12" si="3">+M12*N12</f>
+        <v>139365680.94</v>
+      </c>
+      <c r="P12" s="8">
+        <v>0.09</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="2"/>
+        <v>627145564.23000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>14500</v>
+      </c>
+      <c r="L13">
+        <v>14500</v>
+      </c>
+      <c r="M13" s="5">
+        <v>6968284047</v>
+      </c>
+      <c r="N13" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="O13" s="10">
+        <f>+M13*N13</f>
+        <v>13936568.094000001</v>
+      </c>
+      <c r="P13" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="2"/>
+        <v>348414202.35000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>71</v>
+      </c>
+      <c r="M14" s="5"/>
+      <c r="N14" s="10">
+        <f>+AVERAGE(K6:L6)*N6+AVERAGE(K7:L7)*N7+AVERAGE(K8:L8)*N8+AVERAGE(K9:L9)*N9+AVERAGE(K10:L10)*N10+AVERAGE(K11:L11)*N11+AVERAGE(K12:L12)*N12+AVERAGE(K13:L13)*N13</f>
+        <v>3303.51</v>
+      </c>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10">
+        <f>+AVERAGE(K6:L6)*P6+AVERAGE(K7:L7)*P7+AVERAGE(K8:L8)*P8+AVERAGE(K9:L9)*P9+AVERAGE(K10:L10)*P10+AVERAGE(K11:L11)*P11+AVERAGE(K12:L12)*P12+AVERAGE(K13:L13)*P13</f>
+        <v>4692.0700000000006</v>
+      </c>
+      <c r="R14" s="10">
+        <f>+AVERAGE(N14:P14)</f>
+        <v>3997.7900000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M15" s="5"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="R15" s="10"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
         <v>66</v>
       </c>
-      <c r="K12" t="s">
-        <v>67</v>
-      </c>
-      <c r="L12" s="5">
+      <c r="L16" t="s">
+        <v>66</v>
+      </c>
+      <c r="M16" t="s">
+        <v>58</v>
+      </c>
+      <c r="N16">
+        <v>2012</v>
+      </c>
+      <c r="P16">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="17" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>9999</v>
+      </c>
+      <c r="M17" s="5">
         <v>68226787</v>
       </c>
-      <c r="M12" s="6">
+      <c r="N17" s="6">
         <v>0.01</v>
       </c>
-      <c r="N12">
-        <f t="shared" si="1"/>
+      <c r="O17">
+        <f>+M17*N17</f>
         <v>682267.87</v>
       </c>
-      <c r="O12" s="6">
+      <c r="P17" s="6">
         <v>0.01</v>
       </c>
-      <c r="P12">
-        <f t="shared" si="2"/>
+      <c r="Q17">
+        <f>+M17*P17</f>
         <v>682267.87</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" t="s">
-        <v>82</v>
-      </c>
-      <c r="I13" t="s">
-        <v>77</v>
-      </c>
-      <c r="K13" t="s">
+    <row r="18" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>10000</v>
+      </c>
+      <c r="L18">
+        <v>34999</v>
+      </c>
+      <c r="M18" s="5">
+        <v>1268561872</v>
+      </c>
+      <c r="N18" s="6">
+        <v>0.09</v>
+      </c>
+      <c r="O18">
+        <f>+M18*N18</f>
+        <v>114170568.47999999</v>
+      </c>
+      <c r="P18" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="Q18">
+        <f>+M18*P18</f>
+        <v>76113712.319999993</v>
+      </c>
+    </row>
+    <row r="19" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <v>35000</v>
+      </c>
+      <c r="L19">
+        <v>59999</v>
+      </c>
+      <c r="M19" s="5">
+        <v>2243075236</v>
+      </c>
+      <c r="N19" s="6">
+        <v>0.22</v>
+      </c>
+      <c r="O19">
+        <f>+M19*N19</f>
+        <v>493476551.92000002</v>
+      </c>
+      <c r="P19" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="Q19">
+        <f>+M19*P19</f>
+        <v>448615047.20000005</v>
+      </c>
+    </row>
+    <row r="20" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>60000</v>
+      </c>
+      <c r="L20">
+        <v>99999</v>
+      </c>
+      <c r="M20" s="5">
+        <v>3821361703</v>
+      </c>
+      <c r="N20" s="6">
+        <v>0.26</v>
+      </c>
+      <c r="O20">
+        <f>+M20*N20</f>
+        <v>993554042.78000009</v>
+      </c>
+      <c r="P20" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="Q20">
+        <f>+M20*P20</f>
+        <v>878913191.69000006</v>
+      </c>
+    </row>
+    <row r="21" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>100000</v>
+      </c>
+      <c r="L21">
+        <v>199999</v>
+      </c>
+      <c r="M21" s="5">
+        <v>7763260284</v>
+      </c>
+      <c r="N21" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="O21">
+        <f>+M21*N21</f>
+        <v>2406610688.04</v>
+      </c>
+      <c r="P21" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="Q21">
+        <f>+M21*P21</f>
+        <v>3105304113.6000004</v>
+      </c>
+    </row>
+    <row r="22" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>200000</v>
+      </c>
+      <c r="L22">
+        <v>400000</v>
+      </c>
+      <c r="M22" s="5">
+        <v>10901043017</v>
+      </c>
+      <c r="N22" s="6">
+        <v>0.11</v>
+      </c>
+      <c r="O22">
+        <f>+M22*N22</f>
+        <v>1199114731.8700001</v>
+      </c>
+      <c r="P22" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="Q22">
+        <f>+M22*P22</f>
+        <v>1090104301.7</v>
+      </c>
+    </row>
+    <row r="23" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>69</v>
+      </c>
+      <c r="N23" s="10">
+        <f>+AVERAGE(K17:L17)*N17+AVERAGE(K18:L18)*N18+AVERAGE(K19:L19)*N19+AVERAGE(K20:L20)*N20+AVERAGE(K21:L21)*N21+AVERAGE(K22:L22)*N22</f>
+        <v>112824.55499999999</v>
+      </c>
+      <c r="P23" s="10">
+        <f>+AVERAGE(K17:L17)*P17+AVERAGE(K18:L18)*P18+AVERAGE(K19:L19)*P19+AVERAGE(K20:L20)*P20+AVERAGE(K21:L21)*P21+AVERAGE(K22:L22)*P22</f>
+        <v>119299.55</v>
+      </c>
+      <c r="R23" s="10">
+        <f>+AVERAGE(N23:P23)</f>
+        <v>116062.05249999999</v>
+      </c>
+    </row>
+    <row r="24" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="N24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="R24" s="10"/>
+    </row>
+    <row r="25" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>66</v>
+      </c>
+      <c r="L25" t="s">
+        <v>66</v>
+      </c>
+      <c r="M25" t="s">
+        <v>58</v>
+      </c>
+      <c r="N25">
+        <v>2012</v>
+      </c>
+      <c r="P25">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="26" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>4999</v>
+      </c>
+      <c r="N26" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="P26" s="6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="27" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>5000</v>
+      </c>
+      <c r="L27">
+        <v>9999</v>
+      </c>
+      <c r="N27" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="P27" s="6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="28" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>10000</v>
+      </c>
+      <c r="L28">
+        <v>19999</v>
+      </c>
+      <c r="N28" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="P28" s="6">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="29" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>20000</v>
+      </c>
+      <c r="L29">
+        <v>59999</v>
+      </c>
+      <c r="N29" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P29" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K30">
+        <v>60000</v>
+      </c>
+      <c r="L30">
+        <v>79999</v>
+      </c>
+      <c r="N30" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P30" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <v>80000</v>
+      </c>
+      <c r="L31">
+        <v>119999</v>
+      </c>
+      <c r="N31" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="P31" s="6">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="32" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K32">
+        <v>120000</v>
+      </c>
+      <c r="L32">
+        <v>199999</v>
+      </c>
+      <c r="N32" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="P32" s="6">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="33" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K33">
+        <v>200000</v>
+      </c>
+      <c r="L33">
+        <v>200000</v>
+      </c>
+      <c r="N33" s="6">
+        <v>0.43</v>
+      </c>
+      <c r="P33" s="6">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="34" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J34" t="s">
+        <v>69</v>
+      </c>
+      <c r="N34" s="10">
+        <f>+AVERAGE(K26:L26)*N26+AVERAGE(K27:L27)*N27+AVERAGE(K28:L28)*N28+AVERAGE(K29:L29)*N29+AVERAGE(K30:L30)*N30+AVERAGE(K31:L31)*N31+AVERAGE(K32:L32)*N32+AVERAGE(K33:L33)*N33</f>
+        <v>144149.715</v>
+      </c>
+      <c r="P34" s="10">
+        <f>+AVERAGE(K26:L26)*P26+AVERAGE(K27:L27)*P27+AVERAGE(K28:L28)*P28+AVERAGE(K29:L29)*P29+AVERAGE(K30:L30)*P30+AVERAGE(K31:L31)*P31+AVERAGE(K32:L32)*P32+AVERAGE(K33:L33)*P33</f>
+        <v>144149.715</v>
+      </c>
+      <c r="R34" s="10">
+        <f>+AVERAGE(N34:P34)</f>
+        <v>144149.715</v>
+      </c>
+    </row>
+    <row r="35" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="N35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="R35" s="10"/>
+    </row>
+    <row r="36" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>66</v>
+      </c>
+      <c r="L36" t="s">
+        <v>66</v>
+      </c>
+      <c r="M36" t="s">
+        <v>58</v>
+      </c>
+      <c r="N36" t="s">
         <v>68</v>
       </c>
-      <c r="L13" s="5">
-        <v>1268561872</v>
-      </c>
-      <c r="M13" s="6">
-        <v>0.09</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="1"/>
-        <v>114170568.47999999</v>
-      </c>
-      <c r="O13" s="6">
-        <v>0.06</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="2"/>
-        <v>76113712.319999993</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K14" t="s">
+      <c r="O36" t="s">
         <v>69</v>
       </c>
-      <c r="L14" s="5">
-        <v>2243075236</v>
-      </c>
-      <c r="M14" s="6">
-        <v>0.22</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="1"/>
-        <v>493476551.92000002</v>
-      </c>
-      <c r="O14" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="2"/>
-        <v>448615047.20000005</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K15" t="s">
+      <c r="P36" t="s">
         <v>70</v>
       </c>
-      <c r="L15" s="5">
-        <v>3821361703</v>
-      </c>
-      <c r="M15" s="6">
-        <v>0.26</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="1"/>
-        <v>993554042.78000009</v>
-      </c>
-      <c r="O15" s="6">
-        <v>0.23</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="2"/>
-        <v>878913191.69000006</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K16" t="s">
-        <v>71</v>
-      </c>
-      <c r="L16" s="5">
-        <v>7763260284</v>
-      </c>
-      <c r="M16" s="6">
-        <v>0.31</v>
-      </c>
-      <c r="N16">
-        <f>+L16*M16</f>
-        <v>2406610688.04</v>
-      </c>
-      <c r="O16" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="2"/>
-        <v>3105304113.6000004</v>
-      </c>
-    </row>
-    <row r="17" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="K17" t="s">
+    </row>
+    <row r="37" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J37" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>4999</v>
+      </c>
+      <c r="M37">
+        <v>76945792</v>
+      </c>
+      <c r="N37">
+        <v>11620</v>
+      </c>
+      <c r="O37">
+        <v>1925</v>
+      </c>
+      <c r="P37">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="38" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <v>5000</v>
+      </c>
+      <c r="L38">
+        <v>9999</v>
+      </c>
+      <c r="M38">
+        <v>365344150</v>
+      </c>
+      <c r="N38">
+        <v>2894</v>
+      </c>
+      <c r="O38">
+        <v>7339</v>
+      </c>
+      <c r="P38">
+        <v>3320</v>
+      </c>
+    </row>
+    <row r="39" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K39">
+        <v>10000</v>
+      </c>
+      <c r="M39">
+        <v>866510887</v>
+      </c>
+      <c r="N39">
+        <v>1972</v>
+      </c>
+      <c r="O39">
+        <v>22472</v>
+      </c>
+      <c r="P39">
+        <v>7418</v>
+      </c>
+    </row>
+    <row r="40" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
         <v>72</v>
       </c>
-      <c r="L17" s="5">
-        <v>10901043017</v>
-      </c>
-      <c r="M17" s="6">
-        <v>0.11</v>
-      </c>
-      <c r="N17">
-        <f>+L17*M17</f>
-        <v>1199114731.8700001</v>
-      </c>
-      <c r="O17" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="2"/>
-        <v>1090104301.7</v>
-      </c>
-    </row>
-    <row r="18" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="J18" t="s">
-        <v>73</v>
-      </c>
-      <c r="K18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="K19" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="10:16" x14ac:dyDescent="0.25">
-      <c r="K20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="45" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
-      <c r="R45" s="2"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="2"/>
-      <c r="U45" s="2"/>
-      <c r="V45" s="2"/>
-      <c r="W45" s="2"/>
-      <c r="X45" s="2"/>
-      <c r="Y45" s="2"/>
-      <c r="Z45" s="2"/>
-      <c r="AA45" s="2"/>
-      <c r="AB45" s="2"/>
-      <c r="AC45" s="2"/>
-      <c r="AD45" s="2"/>
-      <c r="AE45" s="2"/>
-      <c r="AF45" s="2"/>
-      <c r="AG45" s="2"/>
-      <c r="AH45" s="2"/>
-      <c r="AI45" s="2"/>
-      <c r="AJ45" s="2"/>
-    </row>
-    <row r="46" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4"/>
-      <c r="Q46" s="4"/>
-      <c r="R46" s="4"/>
-      <c r="S46" s="4"/>
-      <c r="T46" s="4"/>
-      <c r="U46" s="4"/>
-      <c r="V46" s="4"/>
-      <c r="W46" s="4"/>
-      <c r="X46" s="4"/>
-      <c r="Y46" s="4"/>
-      <c r="Z46" s="4"/>
-      <c r="AA46" s="4"/>
-      <c r="AB46" s="4"/>
-      <c r="AC46" s="4"/>
-      <c r="AD46" s="4"/>
-      <c r="AE46" s="4"/>
-      <c r="AF46" s="4"/>
-      <c r="AG46" s="4"/>
-      <c r="AH46" s="4"/>
-      <c r="AI46" s="4"/>
-      <c r="AJ46" s="4"/>
-    </row>
-    <row r="47" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
-      <c r="T47" s="4"/>
-      <c r="U47" s="4"/>
-      <c r="V47" s="4"/>
-      <c r="W47" s="4"/>
-      <c r="X47" s="4"/>
-      <c r="Y47" s="4"/>
-      <c r="Z47" s="4"/>
-      <c r="AA47" s="4"/>
-      <c r="AB47" s="4"/>
-      <c r="AC47" s="4"/>
-      <c r="AD47" s="4"/>
-      <c r="AE47" s="4"/>
-      <c r="AF47" s="4"/>
-      <c r="AG47" s="4"/>
-      <c r="AH47" s="4"/>
-      <c r="AI47" s="4"/>
-      <c r="AJ47" s="4"/>
-    </row>
-    <row r="48" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4"/>
-      <c r="Q48" s="4"/>
-      <c r="R48" s="4"/>
-      <c r="S48" s="4"/>
-      <c r="T48" s="4"/>
-      <c r="U48" s="4"/>
-      <c r="V48" s="4"/>
-      <c r="W48" s="4"/>
-      <c r="X48" s="4"/>
-      <c r="Y48" s="4"/>
-      <c r="Z48" s="4"/>
-      <c r="AA48" s="4"/>
-      <c r="AB48" s="4"/>
-      <c r="AC48" s="4"/>
-      <c r="AD48" s="4"/>
-      <c r="AE48" s="4"/>
-      <c r="AF48" s="4"/>
-      <c r="AG48" s="4"/>
-      <c r="AH48" s="4"/>
-      <c r="AI48" s="4"/>
-      <c r="AJ48" s="4"/>
-    </row>
-    <row r="49" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
-      <c r="S49" s="4"/>
-      <c r="T49" s="4"/>
-      <c r="U49" s="4"/>
-      <c r="V49" s="4"/>
-      <c r="W49" s="4"/>
-      <c r="X49" s="4"/>
-      <c r="Y49" s="4"/>
-      <c r="Z49" s="4"/>
-      <c r="AA49" s="4"/>
-      <c r="AB49" s="4"/>
-      <c r="AC49" s="4"/>
-      <c r="AD49" s="4"/>
-      <c r="AE49" s="4"/>
-      <c r="AF49" s="4"/>
-      <c r="AG49" s="4"/>
-      <c r="AH49" s="4"/>
-      <c r="AI49" s="4"/>
-      <c r="AJ49" s="4"/>
-    </row>
-    <row r="50" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-      <c r="P50" s="4"/>
-      <c r="Q50" s="4"/>
-      <c r="R50" s="4"/>
-      <c r="S50" s="4"/>
-      <c r="T50" s="4"/>
-      <c r="U50" s="4"/>
-      <c r="V50" s="4"/>
-      <c r="W50" s="4"/>
-      <c r="X50" s="4"/>
-      <c r="Y50" s="4"/>
-      <c r="Z50" s="4"/>
-      <c r="AA50" s="4"/>
-      <c r="AB50" s="4"/>
-      <c r="AC50" s="4"/>
-      <c r="AD50" s="4"/>
-      <c r="AE50" s="4"/>
-      <c r="AF50" s="4"/>
-      <c r="AG50" s="4"/>
-      <c r="AH50" s="4"/>
-      <c r="AI50" s="4"/>
-      <c r="AJ50" s="4"/>
-    </row>
-    <row r="51" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="O40" s="10">
+        <f>+(N37/SUM(N37:N39))*O37+(N38/SUM(N37:N39))*O38+(N39/SUM(N37:N39))*O39</f>
+        <v>5333.1523717093296</v>
+      </c>
+      <c r="P40" s="10">
+        <f>+(N37/SUM(N37:N39))*P37+(N38/SUM(N37:N39))*P38+(N39/SUM(N37:N39))*P39</f>
+        <v>2258.8351328399854</v>
+      </c>
+    </row>
+    <row r="50" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+      <c r="O50" s="2"/>
+      <c r="P50" s="2"/>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="2"/>
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+      <c r="U50" s="2"/>
+      <c r="V50" s="2"/>
+      <c r="W50" s="2"/>
+      <c r="X50" s="2"/>
+      <c r="Y50" s="2"/>
+      <c r="Z50" s="2"/>
+      <c r="AA50" s="2"/>
+      <c r="AB50" s="2"/>
+      <c r="AC50" s="2"/>
+      <c r="AD50" s="2"/>
+      <c r="AE50" s="2"/>
+      <c r="AF50" s="2"/>
+      <c r="AG50" s="2"/>
+      <c r="AH50" s="2"/>
+      <c r="AI50" s="2"/>
+      <c r="AJ50" s="2"/>
+      <c r="AK50" s="2"/>
+    </row>
+    <row r="51" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
@@ -1666,8 +1781,9 @@
       <c r="AH51" s="4"/>
       <c r="AI51" s="4"/>
       <c r="AJ51" s="4"/>
-    </row>
-    <row r="52" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK51" s="4"/>
+    </row>
+    <row r="52" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
@@ -1703,8 +1819,9 @@
       <c r="AH52" s="4"/>
       <c r="AI52" s="4"/>
       <c r="AJ52" s="4"/>
-    </row>
-    <row r="53" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK52" s="4"/>
+    </row>
+    <row r="53" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
@@ -1740,8 +1857,9 @@
       <c r="AH53" s="4"/>
       <c r="AI53" s="4"/>
       <c r="AJ53" s="4"/>
-    </row>
-    <row r="54" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK53" s="4"/>
+    </row>
+    <row r="54" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
@@ -1777,8 +1895,9 @@
       <c r="AH54" s="4"/>
       <c r="AI54" s="4"/>
       <c r="AJ54" s="4"/>
-    </row>
-    <row r="55" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK54" s="4"/>
+    </row>
+    <row r="55" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
@@ -1814,8 +1933,9 @@
       <c r="AH55" s="4"/>
       <c r="AI55" s="4"/>
       <c r="AJ55" s="4"/>
-    </row>
-    <row r="56" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK55" s="4"/>
+    </row>
+    <row r="56" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
@@ -1851,8 +1971,9 @@
       <c r="AH56" s="4"/>
       <c r="AI56" s="4"/>
       <c r="AJ56" s="4"/>
-    </row>
-    <row r="57" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK56" s="4"/>
+    </row>
+    <row r="57" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
@@ -1888,8 +2009,9 @@
       <c r="AH57" s="4"/>
       <c r="AI57" s="4"/>
       <c r="AJ57" s="4"/>
-    </row>
-    <row r="58" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK57" s="4"/>
+    </row>
+    <row r="58" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
@@ -1925,8 +2047,9 @@
       <c r="AH58" s="4"/>
       <c r="AI58" s="4"/>
       <c r="AJ58" s="4"/>
-    </row>
-    <row r="59" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK58" s="4"/>
+    </row>
+    <row r="59" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -1962,8 +2085,9 @@
       <c r="AH59" s="4"/>
       <c r="AI59" s="4"/>
       <c r="AJ59" s="4"/>
-    </row>
-    <row r="60" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK59" s="4"/>
+    </row>
+    <row r="60" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
@@ -1999,8 +2123,9 @@
       <c r="AH60" s="4"/>
       <c r="AI60" s="4"/>
       <c r="AJ60" s="4"/>
-    </row>
-    <row r="61" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK60" s="4"/>
+    </row>
+    <row r="61" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -2036,8 +2161,9 @@
       <c r="AH61" s="4"/>
       <c r="AI61" s="4"/>
       <c r="AJ61" s="4"/>
-    </row>
-    <row r="62" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK61" s="4"/>
+    </row>
+    <row r="62" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
@@ -2073,8 +2199,9 @@
       <c r="AH62" s="4"/>
       <c r="AI62" s="4"/>
       <c r="AJ62" s="4"/>
-    </row>
-    <row r="63" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK62" s="4"/>
+    </row>
+    <row r="63" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
@@ -2110,8 +2237,9 @@
       <c r="AH63" s="4"/>
       <c r="AI63" s="4"/>
       <c r="AJ63" s="4"/>
-    </row>
-    <row r="64" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK63" s="4"/>
+    </row>
+    <row r="64" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
@@ -2147,8 +2275,9 @@
       <c r="AH64" s="4"/>
       <c r="AI64" s="4"/>
       <c r="AJ64" s="4"/>
-    </row>
-    <row r="65" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK64" s="4"/>
+    </row>
+    <row r="65" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
@@ -2184,8 +2313,9 @@
       <c r="AH65" s="4"/>
       <c r="AI65" s="4"/>
       <c r="AJ65" s="4"/>
-    </row>
-    <row r="66" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK65" s="4"/>
+    </row>
+    <row r="66" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
@@ -2221,8 +2351,9 @@
       <c r="AH66" s="4"/>
       <c r="AI66" s="4"/>
       <c r="AJ66" s="4"/>
-    </row>
-    <row r="67" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK66" s="4"/>
+    </row>
+    <row r="67" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
@@ -2258,8 +2389,9 @@
       <c r="AH67" s="4"/>
       <c r="AI67" s="4"/>
       <c r="AJ67" s="4"/>
-    </row>
-    <row r="68" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK67" s="4"/>
+    </row>
+    <row r="68" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -2295,8 +2427,9 @@
       <c r="AH68" s="4"/>
       <c r="AI68" s="4"/>
       <c r="AJ68" s="4"/>
-    </row>
-    <row r="69" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK68" s="4"/>
+    </row>
+    <row r="69" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B69" s="4"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
@@ -2332,8 +2465,9 @@
       <c r="AH69" s="4"/>
       <c r="AI69" s="4"/>
       <c r="AJ69" s="4"/>
-    </row>
-    <row r="70" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK69" s="4"/>
+    </row>
+    <row r="70" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
@@ -2369,8 +2503,9 @@
       <c r="AH70" s="4"/>
       <c r="AI70" s="4"/>
       <c r="AJ70" s="4"/>
-    </row>
-    <row r="71" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK70" s="4"/>
+    </row>
+    <row r="71" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
@@ -2406,8 +2541,9 @@
       <c r="AH71" s="4"/>
       <c r="AI71" s="4"/>
       <c r="AJ71" s="4"/>
-    </row>
-    <row r="72" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK71" s="4"/>
+    </row>
+    <row r="72" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
@@ -2443,8 +2579,9 @@
       <c r="AH72" s="4"/>
       <c r="AI72" s="4"/>
       <c r="AJ72" s="4"/>
-    </row>
-    <row r="73" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK72" s="4"/>
+    </row>
+    <row r="73" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
@@ -2480,8 +2617,9 @@
       <c r="AH73" s="4"/>
       <c r="AI73" s="4"/>
       <c r="AJ73" s="4"/>
-    </row>
-    <row r="74" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK73" s="4"/>
+    </row>
+    <row r="74" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
@@ -2517,8 +2655,9 @@
       <c r="AH74" s="4"/>
       <c r="AI74" s="4"/>
       <c r="AJ74" s="4"/>
-    </row>
-    <row r="75" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK74" s="4"/>
+    </row>
+    <row r="75" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
@@ -2554,8 +2693,9 @@
       <c r="AH75" s="4"/>
       <c r="AI75" s="4"/>
       <c r="AJ75" s="4"/>
-    </row>
-    <row r="76" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK75" s="4"/>
+    </row>
+    <row r="76" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
@@ -2591,8 +2731,9 @@
       <c r="AH76" s="4"/>
       <c r="AI76" s="4"/>
       <c r="AJ76" s="4"/>
-    </row>
-    <row r="77" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK76" s="4"/>
+    </row>
+    <row r="77" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
@@ -2628,8 +2769,9 @@
       <c r="AH77" s="4"/>
       <c r="AI77" s="4"/>
       <c r="AJ77" s="4"/>
-    </row>
-    <row r="78" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK77" s="4"/>
+    </row>
+    <row r="78" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
@@ -2665,8 +2807,9 @@
       <c r="AH78" s="4"/>
       <c r="AI78" s="4"/>
       <c r="AJ78" s="4"/>
-    </row>
-    <row r="79" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK78" s="4"/>
+    </row>
+    <row r="79" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
@@ -2702,8 +2845,9 @@
       <c r="AH79" s="4"/>
       <c r="AI79" s="4"/>
       <c r="AJ79" s="4"/>
-    </row>
-    <row r="80" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK79" s="4"/>
+    </row>
+    <row r="80" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -2739,8 +2883,9 @@
       <c r="AH80" s="4"/>
       <c r="AI80" s="4"/>
       <c r="AJ80" s="4"/>
-    </row>
-    <row r="81" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK80" s="4"/>
+    </row>
+    <row r="81" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
@@ -2776,8 +2921,9 @@
       <c r="AH81" s="4"/>
       <c r="AI81" s="4"/>
       <c r="AJ81" s="4"/>
-    </row>
-    <row r="82" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK81" s="4"/>
+    </row>
+    <row r="82" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
@@ -2813,8 +2959,9 @@
       <c r="AH82" s="4"/>
       <c r="AI82" s="4"/>
       <c r="AJ82" s="4"/>
-    </row>
-    <row r="83" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK82" s="4"/>
+    </row>
+    <row r="83" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
@@ -2850,8 +2997,9 @@
       <c r="AH83" s="4"/>
       <c r="AI83" s="4"/>
       <c r="AJ83" s="4"/>
-    </row>
-    <row r="84" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK83" s="4"/>
+    </row>
+    <row r="84" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
@@ -2887,8 +3035,9 @@
       <c r="AH84" s="4"/>
       <c r="AI84" s="4"/>
       <c r="AJ84" s="4"/>
-    </row>
-    <row r="85" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK84" s="4"/>
+    </row>
+    <row r="85" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
@@ -2924,8 +3073,9 @@
       <c r="AH85" s="4"/>
       <c r="AI85" s="4"/>
       <c r="AJ85" s="4"/>
-    </row>
-    <row r="86" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK85" s="4"/>
+    </row>
+    <row r="86" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
@@ -2961,8 +3111,9 @@
       <c r="AH86" s="4"/>
       <c r="AI86" s="4"/>
       <c r="AJ86" s="4"/>
-    </row>
-    <row r="87" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK86" s="4"/>
+    </row>
+    <row r="87" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
@@ -2998,8 +3149,9 @@
       <c r="AH87" s="4"/>
       <c r="AI87" s="4"/>
       <c r="AJ87" s="4"/>
-    </row>
-    <row r="88" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK87" s="4"/>
+    </row>
+    <row r="88" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
@@ -3035,8 +3187,9 @@
       <c r="AH88" s="4"/>
       <c r="AI88" s="4"/>
       <c r="AJ88" s="4"/>
-    </row>
-    <row r="89" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK88" s="4"/>
+    </row>
+    <row r="89" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
@@ -3072,8 +3225,9 @@
       <c r="AH89" s="4"/>
       <c r="AI89" s="4"/>
       <c r="AJ89" s="4"/>
-    </row>
-    <row r="90" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK89" s="4"/>
+    </row>
+    <row r="90" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
@@ -3109,8 +3263,9 @@
       <c r="AH90" s="4"/>
       <c r="AI90" s="4"/>
       <c r="AJ90" s="4"/>
-    </row>
-    <row r="91" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK90" s="4"/>
+    </row>
+    <row r="91" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
@@ -3146,8 +3301,9 @@
       <c r="AH91" s="4"/>
       <c r="AI91" s="4"/>
       <c r="AJ91" s="4"/>
-    </row>
-    <row r="92" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK91" s="4"/>
+    </row>
+    <row r="92" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
@@ -3183,8 +3339,9 @@
       <c r="AH92" s="4"/>
       <c r="AI92" s="4"/>
       <c r="AJ92" s="4"/>
-    </row>
-    <row r="93" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK92" s="4"/>
+    </row>
+    <row r="93" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
@@ -3220,8 +3377,9 @@
       <c r="AH93" s="4"/>
       <c r="AI93" s="4"/>
       <c r="AJ93" s="4"/>
-    </row>
-    <row r="94" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK93" s="4"/>
+    </row>
+    <row r="94" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
@@ -3257,8 +3415,9 @@
       <c r="AH94" s="4"/>
       <c r="AI94" s="4"/>
       <c r="AJ94" s="4"/>
-    </row>
-    <row r="95" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK94" s="4"/>
+    </row>
+    <row r="95" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
@@ -3294,8 +3453,9 @@
       <c r="AH95" s="4"/>
       <c r="AI95" s="4"/>
       <c r="AJ95" s="4"/>
-    </row>
-    <row r="96" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK95" s="4"/>
+    </row>
+    <row r="96" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
@@ -3331,8 +3491,9 @@
       <c r="AH96" s="4"/>
       <c r="AI96" s="4"/>
       <c r="AJ96" s="4"/>
-    </row>
-    <row r="97" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK96" s="4"/>
+    </row>
+    <row r="97" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
@@ -3368,8 +3529,9 @@
       <c r="AH97" s="4"/>
       <c r="AI97" s="4"/>
       <c r="AJ97" s="4"/>
-    </row>
-    <row r="98" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK97" s="4"/>
+    </row>
+    <row r="98" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
@@ -3405,8 +3567,9 @@
       <c r="AH98" s="4"/>
       <c r="AI98" s="4"/>
       <c r="AJ98" s="4"/>
-    </row>
-    <row r="99" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK98" s="4"/>
+    </row>
+    <row r="99" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
@@ -3442,8 +3605,9 @@
       <c r="AH99" s="4"/>
       <c r="AI99" s="4"/>
       <c r="AJ99" s="4"/>
-    </row>
-    <row r="100" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK99" s="4"/>
+    </row>
+    <row r="100" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
@@ -3479,8 +3643,9 @@
       <c r="AH100" s="4"/>
       <c r="AI100" s="4"/>
       <c r="AJ100" s="4"/>
-    </row>
-    <row r="101" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK100" s="4"/>
+    </row>
+    <row r="101" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
@@ -3516,8 +3681,9 @@
       <c r="AH101" s="4"/>
       <c r="AI101" s="4"/>
       <c r="AJ101" s="4"/>
-    </row>
-    <row r="102" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK101" s="4"/>
+    </row>
+    <row r="102" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
@@ -3553,8 +3719,9 @@
       <c r="AH102" s="4"/>
       <c r="AI102" s="4"/>
       <c r="AJ102" s="4"/>
-    </row>
-    <row r="103" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK102" s="4"/>
+    </row>
+    <row r="103" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
@@ -3590,8 +3757,9 @@
       <c r="AH103" s="4"/>
       <c r="AI103" s="4"/>
       <c r="AJ103" s="4"/>
-    </row>
-    <row r="104" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK103" s="4"/>
+    </row>
+    <row r="104" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
@@ -3627,8 +3795,9 @@
       <c r="AH104" s="4"/>
       <c r="AI104" s="4"/>
       <c r="AJ104" s="4"/>
-    </row>
-    <row r="105" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK104" s="4"/>
+    </row>
+    <row r="105" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
@@ -3664,8 +3833,9 @@
       <c r="AH105" s="4"/>
       <c r="AI105" s="4"/>
       <c r="AJ105" s="4"/>
-    </row>
-    <row r="106" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK105" s="4"/>
+    </row>
+    <row r="106" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
@@ -3701,8 +3871,9 @@
       <c r="AH106" s="4"/>
       <c r="AI106" s="4"/>
       <c r="AJ106" s="4"/>
-    </row>
-    <row r="107" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK106" s="4"/>
+    </row>
+    <row r="107" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
@@ -3738,8 +3909,9 @@
       <c r="AH107" s="4"/>
       <c r="AI107" s="4"/>
       <c r="AJ107" s="4"/>
-    </row>
-    <row r="108" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK107" s="4"/>
+    </row>
+    <row r="108" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
@@ -3775,8 +3947,9 @@
       <c r="AH108" s="4"/>
       <c r="AI108" s="4"/>
       <c r="AJ108" s="4"/>
-    </row>
-    <row r="109" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK108" s="4"/>
+    </row>
+    <row r="109" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
@@ -3812,8 +3985,9 @@
       <c r="AH109" s="4"/>
       <c r="AI109" s="4"/>
       <c r="AJ109" s="4"/>
-    </row>
-    <row r="110" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="AK109" s="4"/>
+    </row>
+    <row r="110" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
@@ -3849,6 +4023,197 @@
       <c r="AH110" s="4"/>
       <c r="AI110" s="4"/>
       <c r="AJ110" s="4"/>
+      <c r="AK110" s="4"/>
+    </row>
+    <row r="111" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
+      <c r="E111" s="4"/>
+      <c r="F111" s="4"/>
+      <c r="G111" s="4"/>
+      <c r="H111" s="4"/>
+      <c r="I111" s="4"/>
+      <c r="J111" s="4"/>
+      <c r="K111" s="4"/>
+      <c r="L111" s="4"/>
+      <c r="M111" s="4"/>
+      <c r="N111" s="4"/>
+      <c r="O111" s="4"/>
+      <c r="P111" s="4"/>
+      <c r="Q111" s="4"/>
+      <c r="R111" s="4"/>
+      <c r="S111" s="4"/>
+      <c r="T111" s="4"/>
+      <c r="U111" s="4"/>
+      <c r="V111" s="4"/>
+      <c r="W111" s="4"/>
+      <c r="X111" s="4"/>
+      <c r="Y111" s="4"/>
+      <c r="Z111" s="4"/>
+      <c r="AA111" s="4"/>
+      <c r="AB111" s="4"/>
+      <c r="AC111" s="4"/>
+      <c r="AD111" s="4"/>
+      <c r="AE111" s="4"/>
+      <c r="AF111" s="4"/>
+      <c r="AG111" s="4"/>
+      <c r="AH111" s="4"/>
+      <c r="AI111" s="4"/>
+      <c r="AJ111" s="4"/>
+      <c r="AK111" s="4"/>
+    </row>
+    <row r="112" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B112" s="4"/>
+      <c r="C112" s="4"/>
+      <c r="D112" s="4"/>
+      <c r="E112" s="4"/>
+      <c r="F112" s="4"/>
+      <c r="G112" s="4"/>
+      <c r="H112" s="4"/>
+      <c r="I112" s="4"/>
+      <c r="J112" s="4"/>
+      <c r="K112" s="4"/>
+      <c r="L112" s="4"/>
+      <c r="M112" s="4"/>
+      <c r="N112" s="4"/>
+      <c r="O112" s="4"/>
+      <c r="P112" s="4"/>
+      <c r="Q112" s="4"/>
+      <c r="R112" s="4"/>
+      <c r="S112" s="4"/>
+      <c r="T112" s="4"/>
+      <c r="U112" s="4"/>
+      <c r="V112" s="4"/>
+      <c r="W112" s="4"/>
+      <c r="X112" s="4"/>
+      <c r="Y112" s="4"/>
+      <c r="Z112" s="4"/>
+      <c r="AA112" s="4"/>
+      <c r="AB112" s="4"/>
+      <c r="AC112" s="4"/>
+      <c r="AD112" s="4"/>
+      <c r="AE112" s="4"/>
+      <c r="AF112" s="4"/>
+      <c r="AG112" s="4"/>
+      <c r="AH112" s="4"/>
+      <c r="AI112" s="4"/>
+      <c r="AJ112" s="4"/>
+      <c r="AK112" s="4"/>
+    </row>
+    <row r="113" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
+      <c r="D113" s="4"/>
+      <c r="E113" s="4"/>
+      <c r="F113" s="4"/>
+      <c r="G113" s="4"/>
+      <c r="H113" s="4"/>
+      <c r="I113" s="4"/>
+      <c r="J113" s="4"/>
+      <c r="K113" s="4"/>
+      <c r="L113" s="4"/>
+      <c r="M113" s="4"/>
+      <c r="N113" s="4"/>
+      <c r="O113" s="4"/>
+      <c r="P113" s="4"/>
+      <c r="Q113" s="4"/>
+      <c r="R113" s="4"/>
+      <c r="S113" s="4"/>
+      <c r="T113" s="4"/>
+      <c r="U113" s="4"/>
+      <c r="V113" s="4"/>
+      <c r="W113" s="4"/>
+      <c r="X113" s="4"/>
+      <c r="Y113" s="4"/>
+      <c r="Z113" s="4"/>
+      <c r="AA113" s="4"/>
+      <c r="AB113" s="4"/>
+      <c r="AC113" s="4"/>
+      <c r="AD113" s="4"/>
+      <c r="AE113" s="4"/>
+      <c r="AF113" s="4"/>
+      <c r="AG113" s="4"/>
+      <c r="AH113" s="4"/>
+      <c r="AI113" s="4"/>
+      <c r="AJ113" s="4"/>
+      <c r="AK113" s="4"/>
+    </row>
+    <row r="114" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B114" s="4"/>
+      <c r="C114" s="4"/>
+      <c r="D114" s="4"/>
+      <c r="E114" s="4"/>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4"/>
+      <c r="H114" s="4"/>
+      <c r="I114" s="4"/>
+      <c r="J114" s="4"/>
+      <c r="K114" s="4"/>
+      <c r="L114" s="4"/>
+      <c r="M114" s="4"/>
+      <c r="N114" s="4"/>
+      <c r="O114" s="4"/>
+      <c r="P114" s="4"/>
+      <c r="Q114" s="4"/>
+      <c r="R114" s="4"/>
+      <c r="S114" s="4"/>
+      <c r="T114" s="4"/>
+      <c r="U114" s="4"/>
+      <c r="V114" s="4"/>
+      <c r="W114" s="4"/>
+      <c r="X114" s="4"/>
+      <c r="Y114" s="4"/>
+      <c r="Z114" s="4"/>
+      <c r="AA114" s="4"/>
+      <c r="AB114" s="4"/>
+      <c r="AC114" s="4"/>
+      <c r="AD114" s="4"/>
+      <c r="AE114" s="4"/>
+      <c r="AF114" s="4"/>
+      <c r="AG114" s="4"/>
+      <c r="AH114" s="4"/>
+      <c r="AI114" s="4"/>
+      <c r="AJ114" s="4"/>
+      <c r="AK114" s="4"/>
+    </row>
+    <row r="115" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B115" s="4"/>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="4"/>
+      <c r="H115" s="4"/>
+      <c r="I115" s="4"/>
+      <c r="J115" s="4"/>
+      <c r="K115" s="4"/>
+      <c r="L115" s="4"/>
+      <c r="M115" s="4"/>
+      <c r="N115" s="4"/>
+      <c r="O115" s="4"/>
+      <c r="P115" s="4"/>
+      <c r="Q115" s="4"/>
+      <c r="R115" s="4"/>
+      <c r="S115" s="4"/>
+      <c r="T115" s="4"/>
+      <c r="U115" s="4"/>
+      <c r="V115" s="4"/>
+      <c r="W115" s="4"/>
+      <c r="X115" s="4"/>
+      <c r="Y115" s="4"/>
+      <c r="Z115" s="4"/>
+      <c r="AA115" s="4"/>
+      <c r="AB115" s="4"/>
+      <c r="AC115" s="4"/>
+      <c r="AD115" s="4"/>
+      <c r="AE115" s="4"/>
+      <c r="AF115" s="4"/>
+      <c r="AG115" s="4"/>
+      <c r="AH115" s="4"/>
+      <c r="AI115" s="4"/>
+      <c r="AJ115" s="4"/>
+      <c r="AK115" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4756,7 +5121,7 @@
     </row>
     <row r="13" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -4866,7 +5231,7 @@
     </row>
     <row r="14" spans="2:37" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="C14">
         <v>0</v>

</xml_diff>